<commit_message>
ready for first release - fixed Arduino compiler - more documentation - tested SUM mode on 3 Tiles (physical PCB)
</commit_message>
<xml_diff>
--- a/doc/lut_truth_table.xlsx
+++ b/doc/lut_truth_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FPGA\my-discrete-fpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF23DF0-3BA2-49D3-AA60-C87E72BAFE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1130E7-C2D8-49DD-BA98-99419A2094C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{3D218147-FA5D-4FC2-864A-FAAB782F8933}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D218147-FA5D-4FC2-864A-FAAB782F8933}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>s0</t>
   </si>
@@ -72,15 +72,6 @@
   </si>
   <si>
     <t>0x</t>
-  </si>
-  <si>
-    <t>fizz</t>
-  </si>
-  <si>
-    <t>buzz</t>
-  </si>
-  <si>
-    <t>fizz-buzz</t>
   </si>
 </sst>
 </file>
@@ -612,7 +603,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +731,9 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
       <c r="F6" s="8"/>
       <c r="G6" s="12">
         <v>31</v>
@@ -763,11 +756,11 @@
       </c>
       <c r="M6" s="11">
         <f>E6*K6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="11">
         <f>E6*L6</f>
-        <v>0</v>
+        <v>32768</v>
       </c>
       <c r="O6" s="7"/>
     </row>
@@ -784,7 +777,9 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="12">
         <v>30</v>
@@ -808,11 +803,11 @@
       </c>
       <c r="M7" s="11">
         <f t="shared" ref="M7:M21" si="1">E7*K7</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N7" s="11">
         <f t="shared" ref="N7:N21" si="2">E7*L7</f>
-        <v>0</v>
+        <v>16384</v>
       </c>
       <c r="O7" s="7"/>
     </row>
@@ -829,7 +824,9 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="12">
         <v>29</v>
@@ -853,11 +850,11 @@
       </c>
       <c r="M8" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N8" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
       <c r="O8" s="7"/>
     </row>
@@ -874,10 +871,10 @@
       <c r="D9" s="2">
         <v>1</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8"/>
       <c r="G9" s="12">
         <v>28</v>
       </c>
@@ -900,11 +897,11 @@
       </c>
       <c r="M9" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N9" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4096</v>
       </c>
       <c r="O9" s="7"/>
     </row>
@@ -921,7 +918,9 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="12">
         <v>27</v>
@@ -945,11 +944,11 @@
       </c>
       <c r="M10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N10" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2048</v>
       </c>
       <c r="O10" s="7"/>
     </row>
@@ -969,9 +968,7 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="12">
         <v>26</v>
       </c>
@@ -1015,7 +1012,9 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
       <c r="F12" s="8"/>
       <c r="G12" s="12">
         <v>25</v>
@@ -1039,11 +1038,11 @@
       </c>
       <c r="M12" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="N12" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="O12" s="7"/>
     </row>
@@ -1060,7 +1059,9 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
       <c r="F13" s="8"/>
       <c r="G13" s="12">
         <v>24</v>
@@ -1084,11 +1085,11 @@
       </c>
       <c r="M13" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="N13" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="O13" s="7"/>
     </row>
@@ -1151,9 +1152,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="F15" s="8"/>
       <c r="G15" s="12">
         <v>22</v>
       </c>
@@ -1197,12 +1196,8 @@
       <c r="D16" s="2">
         <v>0</v>
       </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="12">
         <v>21</v>
       </c>
@@ -1225,11 +1220,11 @@
       </c>
       <c r="M16" s="11">
         <f t="shared" si="1"/>
-        <v>1024</v>
+        <v>0</v>
       </c>
       <c r="N16" s="11">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="O16" s="7"/>
     </row>
@@ -1292,9 +1287,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="F18" s="8"/>
       <c r="G18" s="12">
         <v>19</v>
       </c>
@@ -1428,12 +1421,8 @@
       <c r="D21" s="2">
         <v>1</v>
       </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="12">
         <v>16</v>
       </c>
@@ -1455,11 +1444,11 @@
       </c>
       <c r="M21" s="11">
         <f t="shared" si="1"/>
-        <v>32768</v>
+        <v>0</v>
       </c>
       <c r="N21" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" s="7"/>
     </row>
@@ -1478,11 +1467,11 @@
       <c r="L22" s="7"/>
       <c r="M22" s="11">
         <f>SUM(M6:M21)</f>
-        <v>33824</v>
+        <v>255</v>
       </c>
       <c r="N22" s="11">
         <f>SUM(N6:N21)</f>
-        <v>1057</v>
+        <v>65280</v>
       </c>
       <c r="O22" s="7"/>
     </row>
@@ -1495,7 +1484,7 @@
       </c>
       <c r="E23" s="6" t="str">
         <f>DEC2HEX(M22)</f>
-        <v>8420</v>
+        <v>FF</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -1517,7 +1506,7 @@
       </c>
       <c r="E24" s="17" t="str">
         <f>DEC2HEX(N22)</f>
-        <v>421</v>
+        <v>FF00</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>

</xml_diff>